<commit_message>
Added example of generating report in XML format from beans collection dataset.
</commit_message>
<xml_diff>
--- a/out/reports/xlsx/report-from-beans-dataset.xlsx
+++ b/out/reports/xlsx/report-from-beans-dataset.xlsx
@@ -494,7 +494,7 @@
       <c r="D9" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.5205</t>
+            <t xml:space="preserve">0.2343</t>
           </r>
         </is>
       </c>
@@ -502,7 +502,7 @@
       <c r="F9" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.1084</t>
+            <t xml:space="preserve">0.5932</t>
           </r>
         </is>
       </c>
@@ -544,7 +544,7 @@
       <c r="D11" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.5040</t>
+            <t xml:space="preserve">0.4896</t>
           </r>
         </is>
       </c>
@@ -552,7 +552,7 @@
       <c r="F11" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.1211</t>
+            <t xml:space="preserve">0.3410</t>
           </r>
         </is>
       </c>
@@ -594,7 +594,7 @@
       <c r="D13" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.3799</t>
+            <t xml:space="preserve">0.2376</t>
           </r>
         </is>
       </c>
@@ -602,7 +602,7 @@
       <c r="F13" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.0223</t>
+            <t xml:space="preserve">0.6916</t>
           </r>
         </is>
       </c>
@@ -644,7 +644,7 @@
       <c r="D15" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.0941</t>
+            <t xml:space="preserve">0.5937</t>
           </r>
         </is>
       </c>
@@ -652,7 +652,7 @@
       <c r="F15" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.2386</t>
+            <t xml:space="preserve">0.3518</t>
           </r>
         </is>
       </c>
@@ -694,7 +694,7 @@
       <c r="D17" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.8705</t>
+            <t xml:space="preserve">0.6982</t>
           </r>
         </is>
       </c>
@@ -702,7 +702,7 @@
       <c r="F17" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.2044</t>
+            <t xml:space="preserve">0.0978</t>
           </r>
         </is>
       </c>
@@ -744,7 +744,7 @@
       <c r="D19" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.4181</t>
+            <t xml:space="preserve">0.4604</t>
           </r>
         </is>
       </c>
@@ -752,7 +752,7 @@
       <c r="F19" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.5792</t>
+            <t xml:space="preserve">0.3871</t>
           </r>
         </is>
       </c>
@@ -794,7 +794,7 @@
       <c r="D21" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.4019</t>
+            <t xml:space="preserve">0.0272</t>
           </r>
         </is>
       </c>
@@ -802,7 +802,7 @@
       <c r="F21" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.5036</t>
+            <t xml:space="preserve">0.9546</t>
           </r>
         </is>
       </c>
@@ -844,7 +844,7 @@
       <c r="D23" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.3386</t>
+            <t xml:space="preserve">0.1985</t>
           </r>
         </is>
       </c>
@@ -852,7 +852,7 @@
       <c r="F23" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.2473</t>
+            <t xml:space="preserve">0.3916</t>
           </r>
         </is>
       </c>
@@ -894,7 +894,7 @@
       <c r="D25" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.0598</t>
+            <t xml:space="preserve">0.8158</t>
           </r>
         </is>
       </c>
@@ -902,7 +902,7 @@
       <c r="F25" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.8335</t>
+            <t xml:space="preserve">0.5864</t>
           </r>
         </is>
       </c>
@@ -944,7 +944,7 @@
       <c r="D27" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.6702</t>
+            <t xml:space="preserve">0.0804</t>
           </r>
         </is>
       </c>
@@ -952,7 +952,7 @@
       <c r="F27" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.0572</t>
+            <t xml:space="preserve">0.9526</t>
           </r>
         </is>
       </c>
@@ -994,7 +994,7 @@
       <c r="D29" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.2163</t>
+            <t xml:space="preserve">0.4208</t>
           </r>
         </is>
       </c>
@@ -1002,7 +1002,7 @@
       <c r="F29" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.9536</t>
+            <t xml:space="preserve">0.0379</t>
           </r>
         </is>
       </c>
@@ -1044,7 +1044,7 @@
       <c r="D31" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.9959</t>
+            <t xml:space="preserve">0.6972</t>
           </r>
         </is>
       </c>
@@ -1052,7 +1052,7 @@
       <c r="F31" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.2905</t>
+            <t xml:space="preserve">0.1794</t>
           </r>
         </is>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="D33" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.9415</t>
+            <t xml:space="preserve">0.2505</t>
           </r>
         </is>
       </c>
@@ -1102,7 +1102,7 @@
       <c r="F33" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.9314</t>
+            <t xml:space="preserve">0.1763</t>
           </r>
         </is>
       </c>
@@ -1144,7 +1144,7 @@
       <c r="D35" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.7694</t>
+            <t xml:space="preserve">0.6450</t>
           </r>
         </is>
       </c>
@@ -1152,7 +1152,7 @@
       <c r="F35" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.7413</t>
+            <t xml:space="preserve">0.5890</t>
           </r>
         </is>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="D37" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.8434</t>
+            <t xml:space="preserve">0.7140</t>
           </r>
         </is>
       </c>
@@ -1202,7 +1202,7 @@
       <c r="F37" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.6666</t>
+            <t xml:space="preserve">0.7115</t>
           </r>
         </is>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="D39" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.3354</t>
+            <t xml:space="preserve">0.2594</t>
           </r>
         </is>
       </c>
@@ -1252,7 +1252,7 @@
       <c r="F39" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.5937</t>
+            <t xml:space="preserve">0.9770</t>
           </r>
         </is>
       </c>
@@ -1294,7 +1294,7 @@
       <c r="D41" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.9375</t>
+            <t xml:space="preserve">0.6945</t>
           </r>
         </is>
       </c>
@@ -1302,7 +1302,7 @@
       <c r="F41" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.4453</t>
+            <t xml:space="preserve">0.7974</t>
           </r>
         </is>
       </c>
@@ -1344,7 +1344,7 @@
       <c r="D43" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.2870</t>
+            <t xml:space="preserve">0.7965</t>
           </r>
         </is>
       </c>
@@ -1352,7 +1352,7 @@
       <c r="F43" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.0725</t>
+            <t xml:space="preserve">0.9127</t>
           </r>
         </is>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="D45" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.1057</t>
+            <t xml:space="preserve">0.6083</t>
           </r>
         </is>
       </c>
@@ -1402,7 +1402,7 @@
       <c r="F45" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.0991</t>
+            <t xml:space="preserve">0.5479</t>
           </r>
         </is>
       </c>
@@ -1444,7 +1444,7 @@
       <c r="D47" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.7220</t>
+            <t xml:space="preserve">0.0027</t>
           </r>
         </is>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="F47" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.7757</t>
+            <t xml:space="preserve">0.2314</t>
           </r>
         </is>
       </c>
@@ -1494,7 +1494,7 @@
       <c r="D49" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.5893</t>
+            <t xml:space="preserve">0.3293</t>
           </r>
         </is>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="F49" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.3117</t>
+            <t xml:space="preserve">0.5688</t>
           </r>
         </is>
       </c>
@@ -1544,7 +1544,7 @@
       <c r="D51" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.5085</t>
+            <t xml:space="preserve">0.3072</t>
           </r>
         </is>
       </c>
@@ -1552,7 +1552,7 @@
       <c r="F51" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.2901</t>
+            <t xml:space="preserve">0.2269</t>
           </r>
         </is>
       </c>
@@ -1594,7 +1594,7 @@
       <c r="D53" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.5621</t>
+            <t xml:space="preserve">0.8420</t>
           </r>
         </is>
       </c>
@@ -1602,7 +1602,7 @@
       <c r="F53" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.3914</t>
+            <t xml:space="preserve">0.0385</t>
           </r>
         </is>
       </c>
@@ -1644,7 +1644,7 @@
       <c r="D55" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.0897</t>
+            <t xml:space="preserve">0.0715</t>
           </r>
         </is>
       </c>
@@ -1652,7 +1652,7 @@
       <c r="F55" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.0138</t>
+            <t xml:space="preserve">0.4508</t>
           </r>
         </is>
       </c>
@@ -1694,7 +1694,7 @@
       <c r="D57" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.3132</t>
+            <t xml:space="preserve">0.1284</t>
           </r>
         </is>
       </c>
@@ -1702,7 +1702,7 @@
       <c r="F57" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.5190</t>
+            <t xml:space="preserve">0.0176</t>
           </r>
         </is>
       </c>
@@ -1744,7 +1744,7 @@
       <c r="D59" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.0514</t>
+            <t xml:space="preserve">0.6429</t>
           </r>
         </is>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="F59" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.4924</t>
+            <t xml:space="preserve">0.5555</t>
           </r>
         </is>
       </c>
@@ -1794,7 +1794,7 @@
       <c r="D61" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.4231</t>
+            <t xml:space="preserve">0.7460</t>
           </r>
         </is>
       </c>
@@ -1802,7 +1802,7 @@
       <c r="F61" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.3251</t>
+            <t xml:space="preserve">0.4122</t>
           </r>
         </is>
       </c>
@@ -1844,7 +1844,7 @@
       <c r="D63" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.7781</t>
+            <t xml:space="preserve">0.6371</t>
           </r>
         </is>
       </c>
@@ -1852,7 +1852,7 @@
       <c r="F63" s="11" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">0.2558</t>
+            <t xml:space="preserve">0.2979</t>
           </r>
         </is>
       </c>

</xml_diff>